<commit_message>
ADDED:FileNotFoundException class and refactored code in ExcelUtil class for writing data into excel sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/Udemy.xlsx
+++ b/src/test/resources/Udemy.xlsx
@@ -11,7 +11,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,33 +19,52 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>venkatasreedevi305@gmail.com</t>
-  </si>
-  <si>
-    <t>sreedevi30</t>
-  </si>
-  <si>
-    <t>sreedevi31</t>
-  </si>
-  <si>
-    <t>sreedevi32</t>
-  </si>
-  <si>
-    <t>sreedevi33</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="13">
+  <si>
+    <t>TestCase Name</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Test Results</t>
+  </si>
+  <si>
+    <t>dineshkumar.icon.dk@gmail.com</t>
+  </si>
+  <si>
+    <t>Dinnu@247</t>
+  </si>
+  <si>
+    <t>Dinnu@248</t>
+  </si>
+  <si>
+    <t>Dinnu@249</t>
+  </si>
+  <si>
+    <t>Dinnu@250</t>
+  </si>
+  <si>
+    <t>loginTo_Application_WithValid_Credentials</t>
+  </si>
+  <si>
+    <t>Skipped</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -63,12 +82,42 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="53"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="53"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -84,9 +133,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -368,64 +446,100 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D2" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="52.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="41.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s" s="27">
+        <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s" s="28">
+        <v>11</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s" s="29">
+        <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>2</v>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s" s="30">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2" display="Dinnu@247"/>
-    <hyperlink ref="A3:A5" r:id="rId3" display="venkatasreedevi305@gmail.com"/>
-    <hyperlink ref="B3:B5" r:id="rId4" display="Dinnu@247"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId3"/>
+    <hyperlink ref="B4" r:id="rId4"/>
+    <hyperlink ref="B5" r:id="rId5"/>
+    <hyperlink ref="C3" r:id="rId6" display="Dinnu@247"/>
+    <hyperlink ref="C4" r:id="rId7" display="Dinnu@247"/>
+    <hyperlink ref="C5" r:id="rId8" display="Dinnu@247"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>